<commit_message>
10/10 SOAP done, fixing REST case Response issues
</commit_message>
<xml_diff>
--- a/src/main/resources/excelsheets/usZip/GetInfoByAreaCode/USAreaCode.xlsx
+++ b/src/main/resources/excelsheets/usZip/GetInfoByAreaCode/USAreaCode.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21975" windowHeight="6990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>main</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Xpath</t>
   </si>
@@ -30,7 +27,37 @@
     <t>Value</t>
   </si>
   <si>
-    <t>/Envelope/Body/GetInfoByAreaCode/USAreaCode</t>
+    <t>[A-Z a-z].*</t>
+  </si>
+  <si>
+    <t>[0-9]{5}</t>
+  </si>
+  <si>
+    <t>[0-9]{3}</t>
+  </si>
+  <si>
+    <t>[A-Z]{1}</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>/Envelope/Body/GetInfoByAreaCodeResponse/GetInfoByAreaCodeResult/NewDataSet/Table[1]/CITY</t>
+  </si>
+  <si>
+    <t>/Envelope/Body/GetInfoByAreaCodeResponse/GetInfoByAreaCodeResult/NewDataSet/Table[1]/STATE</t>
+  </si>
+  <si>
+    <t>/Envelope/Body/GetInfoByAreaCodeResponse/GetInfoByAreaCodeResult/NewDataSet/Table[1]/ZIP</t>
+  </si>
+  <si>
+    <t>/Envelope/Body/GetInfoByAreaCodeResponse/GetInfoByAreaCodeResult/NewDataSet/Table[1]/AREA_CODE</t>
+  </si>
+  <si>
+    <t>/Envelope/Body/GetInfoByAreaCodeResponse/GetInfoByAreaCodeResult/NewDataSet/Table[1]/TIME_ZONE</t>
+  </si>
+  <si>
+    <t>[A-Z]{2}</t>
   </si>
 </sst>
 </file>
@@ -348,31 +375,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>